<commit_message>
Enable importJava and annotationJava on ignoreImport and ignoreAnnotation situations.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectKtAnnotationSample.xlsx
+++ b/meta/objects/BlancoValueObjectKtAnnotationSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObject/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BCD1E5-3413-044D-82BB-2F301C1E850E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220769D0-70F8-9A47-A23B-D1BD9C567BFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9180" yWindow="2100" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="82">
   <si>
     <t>クラス名</t>
   </si>
@@ -440,6 +440,24 @@
     <rPh sb="0" eb="2">
       <t xml:space="preserve">ヒッス </t>
     </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>バリューオブジェクト定義(Java)・インポート</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>@JsonProperty(
+    "option: fuga"
+)</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>@JsonProperty</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>アノテーション(Java)</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -537,7 +555,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -587,15 +605,6 @@
         <color indexed="8"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="8"/>
       </top>
@@ -610,15 +619,6 @@
       <top style="thin">
         <color indexed="8"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -1053,7 +1053,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1063,64 +1063,62 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1128,21 +1126,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1150,29 +1148,29 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="34" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1184,16 +1182,16 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1201,13 +1199,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1222,22 +1220,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1651,10 +1649,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="F22" workbookViewId="0">
+      <selection activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1669,7 +1667,8 @@
     <col min="13" max="13" width="6.83203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="28" style="1" customWidth="1"/>
     <col min="15" max="15" width="33.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9" style="1"/>
+    <col min="16" max="16" width="31.1640625" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19">
@@ -1699,11 +1698,11 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="3" t="s">
@@ -1713,107 +1712,107 @@
       <c r="C6" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="81"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="39"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="37"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="81"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="39"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="79"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="37"/>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="39"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="37"/>
     </row>
     <row r="9" spans="1:14" ht="45">
       <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="84" t="s">
+      <c r="C9" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="81"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="39"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="37"/>
     </row>
     <row r="10" spans="1:14" ht="15">
       <c r="A10" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="84" t="s">
+      <c r="C10" s="82" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="81"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="39"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="37"/>
     </row>
     <row r="11" spans="1:14" ht="29" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="86" t="s">
+      <c r="C11" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="87"/>
-      <c r="E11" s="87"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="82"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="69"/>
-      <c r="K11" s="69"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="85"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="3" t="s">
@@ -1823,42 +1822,42 @@
       <c r="C12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="38"/>
-    </row>
-    <row r="13" spans="1:14" s="33" customFormat="1">
-      <c r="A13" s="66" t="s">
+      <c r="G12" s="79"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+    </row>
+    <row r="13" spans="1:14" s="31" customFormat="1">
+      <c r="A13" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="67"/>
-      <c r="C13" s="68" t="s">
+      <c r="B13" s="65"/>
+      <c r="C13" s="66" t="s">
         <v>74</v>
       </c>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
-      <c r="H13" s="70"/>
-      <c r="I13" s="70"/>
-      <c r="J13" s="70"/>
-      <c r="K13" s="73"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="71"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:14" s="33" customFormat="1">
-      <c r="A14" s="66" t="s">
+    <row r="14" spans="1:14" s="31" customFormat="1">
+      <c r="A14" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="67"/>
-      <c r="C14" s="68" t="s">
+      <c r="B14" s="65"/>
+      <c r="C14" s="66" t="s">
         <v>45</v>
       </c>
       <c r="D14" t="s">
@@ -1867,157 +1866,157 @@
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14"/>
-      <c r="H14" s="70"/>
-      <c r="I14" s="70"/>
-      <c r="J14" s="70"/>
-      <c r="K14" s="73"/>
+      <c r="H14" s="68"/>
+      <c r="I14" s="68"/>
+      <c r="J14" s="68"/>
+      <c r="K14" s="71"/>
       <c r="L14"/>
     </row>
-    <row r="15" spans="1:14" s="33" customFormat="1">
-      <c r="A15" s="66" t="s">
+    <row r="15" spans="1:14" s="31" customFormat="1">
+      <c r="A15" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="67"/>
-      <c r="C15" s="68"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="66"/>
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15"/>
-      <c r="H15" s="70"/>
-      <c r="I15" s="70"/>
-      <c r="J15" s="70"/>
-      <c r="K15" s="73"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="71"/>
       <c r="L15"/>
     </row>
-    <row r="16" spans="1:14" s="33" customFormat="1">
-      <c r="A16" s="66" t="s">
+    <row r="16" spans="1:14" s="31" customFormat="1">
+      <c r="A16" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="67"/>
-      <c r="C16" s="68" t="s">
+      <c r="B16" s="65"/>
+      <c r="C16" s="66" t="s">
         <v>45</v>
       </c>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16"/>
-      <c r="H16" s="70"/>
-      <c r="I16" s="70"/>
-      <c r="J16" s="70"/>
-      <c r="K16" s="73"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="68"/>
+      <c r="J16" s="68"/>
+      <c r="K16" s="71"/>
       <c r="L16"/>
     </row>
-    <row r="17" spans="1:16" s="33" customFormat="1">
-      <c r="A17" s="66" t="s">
+    <row r="17" spans="1:16" s="31" customFormat="1">
+      <c r="A17" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="67"/>
-      <c r="C17" s="68" t="s">
+      <c r="B17" s="65"/>
+      <c r="C17" s="66" t="s">
         <v>45</v>
       </c>
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17"/>
-      <c r="H17" s="70"/>
-      <c r="I17" s="70"/>
-      <c r="J17" s="70"/>
-      <c r="K17" s="73"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="68"/>
+      <c r="K17" s="71"/>
       <c r="L17"/>
     </row>
-    <row r="18" spans="1:16" s="33" customFormat="1">
-      <c r="A18" s="66" t="s">
+    <row r="18" spans="1:16" s="31" customFormat="1">
+      <c r="A18" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="67"/>
-      <c r="C18" s="68" t="s">
+      <c r="B18" s="65"/>
+      <c r="C18" s="66" t="s">
         <v>45</v>
       </c>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
       <c r="G18"/>
-      <c r="H18" s="70"/>
-      <c r="I18" s="70"/>
-      <c r="J18" s="70"/>
-      <c r="K18" s="73"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="71"/>
       <c r="L18"/>
     </row>
-    <row r="19" spans="1:16" s="41" customFormat="1">
-      <c r="A19" s="38"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="38"/>
-      <c r="N19" s="38"/>
+    <row r="19" spans="1:16" s="39" customFormat="1">
+      <c r="A19" s="36"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
     </row>
     <row r="20" spans="1:16">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="48"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33"/>
-      <c r="P20" s="33"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="31"/>
     </row>
     <row r="21" spans="1:16">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="36" t="s">
+      <c r="B21" s="33"/>
+      <c r="C21" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="71"/>
-      <c r="H21" s="71"/>
-      <c r="I21" s="71"/>
-      <c r="J21" s="71"/>
-      <c r="K21" s="71"/>
-      <c r="L21" s="71"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33"/>
-      <c r="P21" s="33"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="69"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="69"/>
+      <c r="K21" s="69"/>
+      <c r="L21" s="69"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="31"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="31"/>
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6"/>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="76"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="39"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="37"/>
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="3" t="s">
@@ -2025,538 +2024,662 @@
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="38"/>
-      <c r="K23" s="38"/>
-      <c r="L23" s="39"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="37"/>
     </row>
     <row r="24" spans="1:16">
-      <c r="A24" s="38"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="38"/>
-      <c r="L24" s="39"/>
+      <c r="A24" s="36"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="37"/>
     </row>
     <row r="25" spans="1:16">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="48"/>
-      <c r="J25" s="48"/>
-      <c r="K25" s="48"/>
-      <c r="L25" s="48"/>
-      <c r="M25" s="47"/>
-      <c r="N25" s="47"/>
-      <c r="O25" s="47"/>
-      <c r="P25" s="47"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="45"/>
+      <c r="N25" s="45"/>
+      <c r="O25" s="45"/>
+      <c r="P25" s="45"/>
     </row>
     <row r="26" spans="1:16">
-      <c r="A26" s="51" t="s">
+      <c r="A26" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="71"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="71"/>
-      <c r="K26" s="71"/>
-      <c r="L26" s="71"/>
-      <c r="M26" s="48"/>
-      <c r="N26" s="49"/>
-      <c r="O26" s="49"/>
-      <c r="P26" s="39"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="69"/>
+      <c r="H26" s="69"/>
+      <c r="I26" s="69"/>
+      <c r="J26" s="69"/>
+      <c r="K26" s="69"/>
+      <c r="L26" s="69"/>
+      <c r="M26" s="46"/>
+      <c r="N26" s="47"/>
+      <c r="O26" s="47"/>
+      <c r="P26" s="37"/>
     </row>
     <row r="27" spans="1:16">
-      <c r="A27" s="55">
+      <c r="A27" s="53">
         <v>1</v>
       </c>
-      <c r="B27" s="50" t="s">
+      <c r="B27" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="72"/>
-      <c r="H27" s="72"/>
-      <c r="I27" s="72"/>
-      <c r="J27" s="72"/>
-      <c r="K27" s="72"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="40"/>
-      <c r="N27" s="40"/>
-      <c r="O27" s="40"/>
-      <c r="P27" s="39"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="70"/>
+      <c r="H27" s="70"/>
+      <c r="I27" s="70"/>
+      <c r="J27" s="70"/>
+      <c r="K27" s="70"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="38"/>
+      <c r="N27" s="38"/>
+      <c r="O27" s="38"/>
+      <c r="P27" s="37"/>
     </row>
     <row r="28" spans="1:16">
-      <c r="A28" s="55"/>
-      <c r="B28" s="50"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="72"/>
-      <c r="H28" s="72"/>
-      <c r="I28" s="72"/>
-      <c r="J28" s="72"/>
-      <c r="K28" s="72"/>
-      <c r="L28" s="38"/>
-      <c r="M28" s="40"/>
-      <c r="N28" s="40"/>
-      <c r="O28" s="40"/>
-      <c r="P28" s="39"/>
+      <c r="A28" s="53"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="70"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="70"/>
+      <c r="J28" s="70"/>
+      <c r="K28" s="70"/>
+      <c r="L28" s="36"/>
+      <c r="M28" s="38"/>
+      <c r="N28" s="38"/>
+      <c r="O28" s="38"/>
+      <c r="P28" s="37"/>
     </row>
     <row r="29" spans="1:16">
-      <c r="A29" s="56"/>
-      <c r="B29" s="52"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="54"/>
-      <c r="G29" s="72"/>
-      <c r="H29" s="72"/>
-      <c r="I29" s="72"/>
-      <c r="J29" s="72"/>
-      <c r="K29" s="72"/>
-      <c r="L29" s="38"/>
-      <c r="M29" s="40"/>
-      <c r="N29" s="40"/>
-      <c r="O29" s="40"/>
-      <c r="P29" s="39"/>
-    </row>
-    <row r="30" spans="1:16" s="41" customFormat="1">
-      <c r="A30" s="38"/>
-      <c r="B30" s="40"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="38"/>
-      <c r="M30" s="38"/>
-      <c r="N30" s="38"/>
+      <c r="A29" s="54"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="70"/>
+      <c r="H29" s="70"/>
+      <c r="I29" s="70"/>
+      <c r="J29" s="70"/>
+      <c r="K29" s="70"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="38"/>
+      <c r="N29" s="38"/>
+      <c r="O29" s="38"/>
+      <c r="P29" s="37"/>
+    </row>
+    <row r="30" spans="1:16" s="39" customFormat="1">
+      <c r="A30" s="36"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="36"/>
+      <c r="M30" s="36"/>
+      <c r="N30" s="36"/>
     </row>
     <row r="31" spans="1:16">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="48"/>
-      <c r="J31" s="48"/>
-      <c r="K31" s="48"/>
-      <c r="L31" s="48"/>
-      <c r="M31" s="47"/>
-      <c r="N31" s="47"/>
-      <c r="O31" s="47"/>
-      <c r="P31" s="47"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="45"/>
+      <c r="N31" s="45"/>
+      <c r="O31" s="45"/>
+      <c r="P31" s="45"/>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="51" t="s">
+      <c r="A32" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="46" t="s">
+      <c r="B32" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="71"/>
-      <c r="H32" s="71"/>
-      <c r="I32" s="71"/>
-      <c r="J32" s="71"/>
-      <c r="K32" s="71"/>
-      <c r="L32" s="71"/>
-      <c r="M32" s="48"/>
-      <c r="N32" s="49"/>
-      <c r="O32" s="49"/>
-      <c r="P32" s="39"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="69"/>
+      <c r="H32" s="69"/>
+      <c r="I32" s="69"/>
+      <c r="J32" s="69"/>
+      <c r="K32" s="69"/>
+      <c r="L32" s="69"/>
+      <c r="M32" s="46"/>
+      <c r="N32" s="47"/>
+      <c r="O32" s="47"/>
+      <c r="P32" s="37"/>
     </row>
     <row r="33" spans="1:16">
-      <c r="A33" s="55">
+      <c r="A33" s="53">
         <v>1</v>
       </c>
-      <c r="B33" s="50" t="s">
+      <c r="B33" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="42"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="72"/>
-      <c r="H33" s="72"/>
-      <c r="I33" s="72"/>
-      <c r="J33" s="72"/>
-      <c r="K33" s="72"/>
-      <c r="L33" s="38"/>
-      <c r="M33" s="40"/>
-      <c r="N33" s="40"/>
-      <c r="O33" s="40"/>
-      <c r="P33" s="39"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="70"/>
+      <c r="H33" s="70"/>
+      <c r="I33" s="70"/>
+      <c r="J33" s="70"/>
+      <c r="K33" s="70"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="38"/>
+      <c r="N33" s="38"/>
+      <c r="O33" s="38"/>
+      <c r="P33" s="37"/>
     </row>
     <row r="34" spans="1:16">
-      <c r="A34" s="55">
+      <c r="A34" s="53">
         <v>2</v>
       </c>
-      <c r="B34" s="50" t="s">
+      <c r="B34" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="44"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="45"/>
-      <c r="G34" s="72"/>
-      <c r="H34" s="72"/>
-      <c r="I34" s="72"/>
-      <c r="J34" s="72"/>
-      <c r="K34" s="72"/>
-      <c r="L34" s="38"/>
-      <c r="M34" s="40"/>
-      <c r="N34" s="40"/>
-      <c r="O34" s="40"/>
-      <c r="P34" s="39"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="70"/>
+      <c r="H34" s="70"/>
+      <c r="I34" s="70"/>
+      <c r="J34" s="70"/>
+      <c r="K34" s="70"/>
+      <c r="L34" s="36"/>
+      <c r="M34" s="38"/>
+      <c r="N34" s="38"/>
+      <c r="O34" s="38"/>
+      <c r="P34" s="37"/>
     </row>
     <row r="35" spans="1:16">
-      <c r="A35" s="56"/>
-      <c r="B35" s="52"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="54"/>
-      <c r="G35" s="72"/>
-      <c r="H35" s="72"/>
-      <c r="I35" s="72"/>
-      <c r="J35" s="72"/>
-      <c r="K35" s="72"/>
-      <c r="L35" s="38"/>
-      <c r="M35" s="40"/>
-      <c r="N35" s="40"/>
-      <c r="O35" s="40"/>
-      <c r="P35" s="39"/>
+      <c r="A35" s="54"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="51"/>
+      <c r="F35" s="52"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="70"/>
+      <c r="I35" s="70"/>
+      <c r="J35" s="70"/>
+      <c r="K35" s="70"/>
+      <c r="L35" s="36"/>
+      <c r="M35" s="38"/>
+      <c r="N35" s="38"/>
+      <c r="O35" s="38"/>
+      <c r="P35" s="37"/>
     </row>
     <row r="36" spans="1:16">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
     </row>
     <row r="37" spans="1:16">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="46"/>
+      <c r="J37" s="46"/>
+      <c r="K37" s="46"/>
+      <c r="L37" s="46"/>
+      <c r="M37" s="45"/>
+      <c r="N37" s="45"/>
+      <c r="O37" s="45"/>
+      <c r="P37" s="45"/>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="A38" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="44"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="69"/>
+      <c r="H38" s="69"/>
+      <c r="I38" s="69"/>
+      <c r="J38" s="69"/>
+      <c r="K38" s="69"/>
+      <c r="L38" s="69"/>
+      <c r="M38" s="46"/>
+      <c r="N38" s="47"/>
+      <c r="O38" s="47"/>
+      <c r="P38" s="37"/>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="A39" s="53">
+        <v>1</v>
+      </c>
+      <c r="B39" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="41"/>
+      <c r="G39" s="70"/>
+      <c r="H39" s="70"/>
+      <c r="I39" s="70"/>
+      <c r="J39" s="70"/>
+      <c r="K39" s="70"/>
+      <c r="L39" s="36"/>
+      <c r="M39" s="38"/>
+      <c r="N39" s="38"/>
+      <c r="O39" s="38"/>
+      <c r="P39" s="37"/>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="A40" s="53"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="70"/>
+      <c r="H40" s="70"/>
+      <c r="I40" s="70"/>
+      <c r="J40" s="70"/>
+      <c r="K40" s="70"/>
+      <c r="L40" s="36"/>
+      <c r="M40" s="38"/>
+      <c r="N40" s="38"/>
+      <c r="O40" s="38"/>
+      <c r="P40" s="37"/>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="A41" s="54"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="52"/>
+      <c r="G41" s="70"/>
+      <c r="H41" s="70"/>
+      <c r="I41" s="70"/>
+      <c r="J41" s="70"/>
+      <c r="K41" s="70"/>
+      <c r="L41" s="36"/>
+      <c r="M41" s="38"/>
+      <c r="N41" s="38"/>
+      <c r="O41" s="38"/>
+      <c r="P41" s="37"/>
+    </row>
+    <row r="42" spans="1:16">
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+      <c r="K42" s="12"/>
+      <c r="L42" s="12"/>
+      <c r="M42" s="12"/>
+    </row>
+    <row r="43" spans="1:16">
+      <c r="A43" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="15"/>
-    </row>
-    <row r="38" spans="1:16" ht="13.5" customHeight="1">
-      <c r="A38" s="90" t="s">
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="6"/>
+      <c r="P43" s="13"/>
+    </row>
+    <row r="44" spans="1:16" ht="13.5" customHeight="1">
+      <c r="A44" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="90" t="s">
+      <c r="B44" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="89" t="s">
+      <c r="C44" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="89" t="s">
+      <c r="D44" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="E38" s="91" t="s">
+      <c r="E44" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="F38" s="89" t="s">
+      <c r="F44" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="G38" s="91" t="s">
+      <c r="G44" s="89" t="s">
         <v>66</v>
       </c>
-      <c r="H38" s="91" t="s">
+      <c r="H44" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="I38" s="94" t="s">
+      <c r="I44" s="92" t="s">
         <v>77</v>
       </c>
-      <c r="J38" s="94" t="s">
+      <c r="J44" s="92" t="s">
         <v>59</v>
       </c>
-      <c r="K38" s="94" t="s">
+      <c r="K44" s="92" t="s">
         <v>58</v>
       </c>
-      <c r="L38" s="89" t="s">
+      <c r="L44" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="M38" s="89"/>
-      <c r="N38" s="16"/>
-      <c r="O38" s="17"/>
-      <c r="P38" s="9"/>
-    </row>
-    <row r="39" spans="1:16">
-      <c r="A39" s="90"/>
-      <c r="B39" s="90"/>
-      <c r="C39" s="89"/>
-      <c r="D39" s="89"/>
-      <c r="E39" s="92"/>
-      <c r="F39" s="89"/>
-      <c r="G39" s="93"/>
-      <c r="H39" s="93"/>
-      <c r="I39" s="95"/>
-      <c r="J39" s="95"/>
-      <c r="K39" s="95"/>
-      <c r="L39" s="89"/>
-      <c r="M39" s="89"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="30"/>
-      <c r="P39" s="15"/>
-    </row>
-    <row r="40" spans="1:16">
-      <c r="A40" s="19">
+      <c r="M44" s="87"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="89" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="A45" s="88"/>
+      <c r="B45" s="88"/>
+      <c r="C45" s="87"/>
+      <c r="D45" s="87"/>
+      <c r="E45" s="90"/>
+      <c r="F45" s="87"/>
+      <c r="G45" s="91"/>
+      <c r="H45" s="91"/>
+      <c r="I45" s="93"/>
+      <c r="J45" s="93"/>
+      <c r="K45" s="93"/>
+      <c r="L45" s="87"/>
+      <c r="M45" s="87"/>
+      <c r="N45" s="16"/>
+      <c r="O45" s="28"/>
+      <c r="P45" s="90"/>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="A46" s="17">
         <v>1</v>
       </c>
-      <c r="B40" s="20" t="s">
+      <c r="B46" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C40" s="21" t="s">
+      <c r="C46" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21" t="s">
+      <c r="D46" s="19"/>
+      <c r="E46" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="F40" s="21" t="s">
+      <c r="F46" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="G40" s="21"/>
-      <c r="H40" s="78" t="s">
+      <c r="G46" s="19"/>
+      <c r="H46" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="I40" s="78" t="s">
+      <c r="I46" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="J40" s="78" t="s">
+      <c r="J46" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="K40" s="78" t="s">
+      <c r="K46" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="L40" s="21" t="s">
+      <c r="L46" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="M40" s="22"/>
-      <c r="N40" s="22"/>
-      <c r="O40" s="29"/>
-      <c r="P40" s="15"/>
-    </row>
-    <row r="41" spans="1:16" ht="60">
-      <c r="A41" s="19">
-        <f>A40+1</f>
+      <c r="M46" s="20"/>
+      <c r="N46" s="20"/>
+      <c r="O46" s="27"/>
+      <c r="P46" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="60">
+      <c r="A47" s="17">
+        <f>A46+1</f>
         <v>2</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B47" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="21" t="s">
+      <c r="C47" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="D41" s="21"/>
-      <c r="E41" s="85" t="s">
+      <c r="D47" s="19"/>
+      <c r="E47" s="83" t="s">
         <v>69</v>
       </c>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="78"/>
-      <c r="I41" s="78"/>
-      <c r="J41" s="78"/>
-      <c r="K41" s="78" t="s">
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="76"/>
+      <c r="I47" s="76"/>
+      <c r="J47" s="76"/>
+      <c r="K47" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="L41" s="21"/>
-      <c r="M41" s="22"/>
-      <c r="N41" s="22"/>
-      <c r="O41" s="29"/>
-      <c r="P41" s="15"/>
-    </row>
-    <row r="42" spans="1:16">
-      <c r="A42" s="19">
-        <f t="shared" ref="A42:A44" si="0">A41+1</f>
+      <c r="L47" s="19"/>
+      <c r="M47" s="20"/>
+      <c r="N47" s="20"/>
+      <c r="O47" s="27"/>
+      <c r="P47" s="83" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
+      <c r="A48" s="17">
+        <f t="shared" ref="A48:A50" si="0">A47+1</f>
         <v>3</v>
       </c>
-      <c r="B42" s="20" t="s">
+      <c r="B48" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="21" t="s">
+      <c r="C48" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D42" s="21" t="s">
+      <c r="D48" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="78" t="s">
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="I42" s="78"/>
-      <c r="J42" s="78"/>
-      <c r="K42" s="78"/>
-      <c r="L42" s="21" t="s">
+      <c r="I48" s="76"/>
+      <c r="J48" s="76"/>
+      <c r="K48" s="76"/>
+      <c r="L48" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="M42" s="22"/>
-      <c r="N42" s="22"/>
-      <c r="O42" s="23"/>
-      <c r="P42" s="15"/>
-    </row>
-    <row r="43" spans="1:16" ht="30">
-      <c r="A43" s="19">
+      <c r="M48" s="20"/>
+      <c r="N48" s="20"/>
+      <c r="O48" s="21"/>
+      <c r="P48" s="19"/>
+    </row>
+    <row r="49" spans="1:16" ht="30">
+      <c r="A49" s="17">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B49" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C43" s="21" t="s">
+      <c r="C49" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D43" s="21"/>
-      <c r="E43" s="85" t="s">
+      <c r="D49" s="19"/>
+      <c r="E49" s="83" t="s">
         <v>67</v>
       </c>
-      <c r="F43" s="21"/>
-      <c r="G43" s="21"/>
-      <c r="H43" s="78"/>
-      <c r="I43" s="78"/>
-      <c r="J43" s="78"/>
-      <c r="K43" s="78"/>
-      <c r="L43" s="21" t="s">
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="76"/>
+      <c r="I49" s="76"/>
+      <c r="J49" s="76"/>
+      <c r="K49" s="76"/>
+      <c r="L49" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="M43" s="22"/>
-      <c r="N43" s="22"/>
-      <c r="O43" s="23"/>
-      <c r="P43" s="15"/>
-    </row>
-    <row r="44" spans="1:16" ht="15">
-      <c r="A44" s="19">
+      <c r="M49" s="20"/>
+      <c r="N49" s="20"/>
+      <c r="O49" s="21"/>
+      <c r="P49" s="83" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="15">
+      <c r="A50" s="17">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B44" s="20" t="s">
+      <c r="B50" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C44" s="21" t="s">
+      <c r="C50" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D44" s="21"/>
-      <c r="E44" s="83" t="s">
+      <c r="D50" s="19"/>
+      <c r="E50" s="81" t="s">
         <v>70</v>
       </c>
-      <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="78"/>
-      <c r="I44" s="78"/>
-      <c r="J44" s="78"/>
-      <c r="K44" s="78"/>
-      <c r="L44" s="21" t="s">
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="76"/>
+      <c r="I50" s="76"/>
+      <c r="J50" s="76"/>
+      <c r="K50" s="76"/>
+      <c r="L50" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="M44" s="22"/>
-      <c r="N44" s="22"/>
-      <c r="O44" s="23"/>
-      <c r="P44" s="15"/>
-    </row>
-    <row r="45" spans="1:16">
-      <c r="A45" s="24"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="26"/>
-      <c r="H45" s="79"/>
-      <c r="I45" s="79"/>
-      <c r="J45" s="79"/>
-      <c r="K45" s="79"/>
-      <c r="L45" s="26"/>
-      <c r="M45" s="27"/>
-      <c r="N45" s="27"/>
-      <c r="O45" s="28"/>
-      <c r="P45" s="15"/>
+      <c r="M50" s="20"/>
+      <c r="N50" s="20"/>
+      <c r="O50" s="21"/>
+      <c r="P50" s="81"/>
+    </row>
+    <row r="51" spans="1:16">
+      <c r="A51" s="22"/>
+      <c r="B51" s="23"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="77"/>
+      <c r="I51" s="77"/>
+      <c r="J51" s="77"/>
+      <c r="K51" s="77"/>
+      <c r="L51" s="24"/>
+      <c r="M51" s="25"/>
+      <c r="N51" s="25"/>
+      <c r="O51" s="26"/>
+      <c r="P51" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="P44:P45"/>
     <mergeCell ref="C11:F11"/>
-    <mergeCell ref="L38:M39"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="K38:K39"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="L44:M45"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="H44:H45"/>
+    <mergeCell ref="K44:K45"/>
+    <mergeCell ref="J44:J45"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="I44:I45"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F61:K61" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F67:K67" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2569,7 +2692,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>accessScope2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15 G40:G45" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15 G46:G51" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>isAbstract</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{061A2328-C320-074B-A7A0-1D5ADA23E625}">
@@ -2591,7 +2714,7 @@
           <x14:formula1>
             <xm:f>config!$P$4:$P$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H40:K45</xm:sqref>
+          <xm:sqref>H46:K51</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2612,107 +2735,107 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="59" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="59" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="59" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" style="59" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="59" customWidth="1"/>
-    <col min="8" max="8" width="9.83203125" style="59" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="59" customWidth="1"/>
-    <col min="10" max="10" width="18.5" style="59" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" style="59" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" style="59" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" style="59" customWidth="1"/>
-    <col min="14" max="14" width="18.6640625" style="59" bestFit="1" customWidth="1"/>
-    <col min="15" max="260" width="8.83203125" style="59" customWidth="1"/>
-    <col min="261" max="16384" width="10.83203125" style="59"/>
+    <col min="1" max="3" width="8.83203125" style="57" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="57" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="57" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" style="57" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="57" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" style="57" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="57" customWidth="1"/>
+    <col min="10" max="10" width="18.5" style="57" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="57" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" style="57" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" style="57" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" style="57" bestFit="1" customWidth="1"/>
+    <col min="15" max="260" width="8.83203125" style="57" customWidth="1"/>
+    <col min="261" max="16384" width="10.83203125" style="57"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="19">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="58" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="58"/>
+      <c r="Q1" s="56"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="60" t="s">
+      <c r="F3" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="60" t="s">
+      <c r="H3" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="60" t="s">
+      <c r="J3" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="60" t="s">
+      <c r="L3" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="60" t="s">
+      <c r="N3" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="P3" s="60" t="s">
+      <c r="P3" s="58" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="B4" s="61"/>
-      <c r="D4" s="64" t="s">
+      <c r="B4" s="59"/>
+      <c r="D4" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="62" t="s">
+      <c r="F4" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="H4" s="62"/>
-      <c r="J4" s="62"/>
-      <c r="L4" s="62"/>
-      <c r="N4" s="62"/>
-      <c r="P4" s="62"/>
+      <c r="H4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="P4" s="60"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="H5" s="64" t="s">
+      <c r="D5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="H5" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="64" t="s">
+      <c r="J5" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="L5" s="64" t="s">
+      <c r="L5" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="N5" s="64" t="s">
+      <c r="N5" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="P5" s="64" t="s">
+      <c r="P5" s="62" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="B6" s="65"/>
+      <c r="B6" s="63"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4"/>

</xml_diff>